<commit_message>
Updated distributions after Week 13
</commit_message>
<xml_diff>
--- a/Base/Teams/49ers/Distributions.xlsx
+++ b/Base/Teams/49ers/Distributions.xlsx
@@ -28,16 +28,16 @@
     <t>PA</t>
   </si>
   <si>
-    <t>NCT(2.801361869810946, 1.5217482927666635, -1.2874023853663543, 2.737176357058992)</t>
-  </si>
-  <si>
-    <t>NIG(1.3638627950358075, 1.0813612211370138, 4.908233950469765, 5.835049805867281)</t>
-  </si>
-  <si>
-    <t>JSU(-0.851550852358577, 1.1518004375718602, 0.6499171194223723, 3.250916149978635)</t>
-  </si>
-  <si>
-    <t>NIG(1.0467644805397178, 0.8072750116586681, 3.515087570847813, 5.833784031249632)</t>
+    <t>NCT(2.799257602882035, 1.5021707826232191, -1.1517886662636974, 2.656790039974177)</t>
+  </si>
+  <si>
+    <t>NIG(1.3972564691830003, 1.1160143088384082, 4.952284557658946, 5.849337751043771)</t>
+  </si>
+  <si>
+    <t>NIG(0.8378493481521685, 0.5587806432168014, 1.3801038347749603, 3.3503922326746287)</t>
+  </si>
+  <si>
+    <t>NCT(2.4556167987130504, 1.51701196430324, -0.009623588115898571, 4.483896015283383)</t>
   </si>
 </sst>
 </file>

</xml_diff>